<commit_message>
WIP Includes insert statements
</commit_message>
<xml_diff>
--- a/datasets/98-Pizza Datasets v170517 copy.xlsx
+++ b/datasets/98-Pizza Datasets v170517 copy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn-daviddaniel/Documents/lgProjects/gc98/98-Pizza/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn-daviddaniel/Documents/lgProjects/gc98/98-Pizza/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="6060" yWindow="-21140" windowWidth="17140" windowHeight="21140" tabRatio="500"/>
-    <workbookView xWindow="-6900" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="500" firstSheet="15" activeTab="16"/>
+    <workbookView xWindow="-6900" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Tables (2)" sheetId="2" r:id="rId1"/>
@@ -4781,7 +4781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
     <sheetView workbookViewId="1">
@@ -6392,7 +6392,9 @@
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D51" sqref="D51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -15353,7 +15355,9 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>